<commit_message>
revisi slip tendik di role admin
</commit_message>
<xml_diff>
--- a/public/contoh-excel/tendik.xlsx
+++ b/public/contoh-excel/tendik.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14025" windowHeight="12150"/>
+    <workbookView windowWidth="28170" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>email</t>
   </si>
@@ -37,16 +37,10 @@
     <t>tunjangan_jabatan</t>
   </si>
   <si>
-    <t>bonus</t>
-  </si>
-  <si>
     <t>tunjangan_kehadiran</t>
   </si>
   <si>
     <t>tunjangan_lembur</t>
-  </si>
-  <si>
-    <t>tunj_pel_mhs_op_feeder</t>
   </si>
   <si>
     <t>tunjangan_kinerja</t>
@@ -90,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -112,23 +106,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,8 +137,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -152,30 +221,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,60 +235,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,43 +251,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,139 +425,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,6 +454,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -471,6 +474,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,41 +523,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,125 +542,114 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
@@ -664,31 +658,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1024,32 +1018,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="9.8" customWidth="true"/>
     <col min="7" max="7" width="14.9" customWidth="true"/>
-    <col min="8" max="8" width="12.5"/>
-    <col min="9" max="9" width="17.7" customWidth="true"/>
-    <col min="10" max="10" width="15" customWidth="true"/>
-    <col min="11" max="11" width="19.2" customWidth="true"/>
-    <col min="12" max="12" width="15.7" customWidth="true"/>
-    <col min="13" max="13" width="16.4" customWidth="true"/>
-    <col min="14" max="14" width="16.2" customWidth="true"/>
-    <col min="15" max="15" width="16.9" customWidth="true"/>
-    <col min="16" max="16" width="17.1" customWidth="true"/>
-    <col min="17" max="17" width="15.8" customWidth="true"/>
-    <col min="18" max="18" width="13.5" customWidth="true"/>
-    <col min="19" max="19" width="16.2" customWidth="true"/>
-    <col min="20" max="20" width="14.3" customWidth="true"/>
+    <col min="8" max="8" width="17.7" customWidth="true"/>
+    <col min="9" max="9" width="15" customWidth="true"/>
+    <col min="10" max="10" width="15.7" customWidth="true"/>
+    <col min="11" max="11" width="16.4" customWidth="true"/>
+    <col min="12" max="12" width="16.2" customWidth="true"/>
+    <col min="13" max="13" width="16.9" customWidth="true"/>
+    <col min="14" max="14" width="17.1" customWidth="true"/>
+    <col min="15" max="15" width="15.8" customWidth="true"/>
+    <col min="16" max="16" width="13.5" customWidth="true"/>
+    <col min="17" max="17" width="16.2" customWidth="true"/>
+    <col min="18" max="18" width="14.3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1104,28 +1096,22 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>2024</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2023</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
       </c>
       <c r="F2">
         <v>255000</v>
@@ -1134,22 +1120,22 @@
         <v>50000</v>
       </c>
       <c r="H2">
-        <v>1600000</v>
+        <v>50000</v>
       </c>
       <c r="I2">
         <v>50000</v>
       </c>
       <c r="J2">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>700000</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1161,15 +1147,9 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>125000</v>
-      </c>
-      <c r="T2">
         <v>125000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update contoh excel tendik
</commit_message>
<xml_diff>
--- a/public/contoh-excel/tendik.xlsx
+++ b/public/contoh-excel/tendik.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>email</t>
   </si>
@@ -40,6 +40,9 @@
     <t>tunjangan_kehadiran</t>
   </si>
   <si>
+    <t>jml_jam_lembur</t>
+  </si>
+  <si>
     <t>tunjangan_lembur</t>
   </si>
   <si>
@@ -70,13 +73,16 @@
     <t>gaji_yang_dibayar</t>
   </si>
   <si>
-    <t>erma@gmail.com</t>
+    <t>erma@primakara.ac.id</t>
   </si>
   <si>
     <t>erma</t>
   </si>
   <si>
     <t>Pengadaan</t>
+  </si>
+  <si>
+    <t>1 jam 30 menit</t>
   </si>
 </sst>
 </file>
@@ -84,10 +90,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -106,11 +112,108 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,53 +225,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,67 +243,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,12 +257,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -269,19 +323,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,145 +431,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +456,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,36 +495,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,147 +533,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1018,30 +1024,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.8" customWidth="true"/>
+    <col min="1" max="1" width="22" customWidth="true"/>
     <col min="7" max="7" width="14.9" customWidth="true"/>
-    <col min="8" max="8" width="17.7" customWidth="true"/>
-    <col min="9" max="9" width="15" customWidth="true"/>
-    <col min="10" max="10" width="15.7" customWidth="true"/>
-    <col min="11" max="11" width="16.4" customWidth="true"/>
-    <col min="12" max="12" width="16.2" customWidth="true"/>
-    <col min="13" max="13" width="16.9" customWidth="true"/>
-    <col min="14" max="14" width="17.1" customWidth="true"/>
-    <col min="15" max="15" width="15.8" customWidth="true"/>
-    <col min="16" max="16" width="13.5" customWidth="true"/>
-    <col min="17" max="17" width="16.2" customWidth="true"/>
-    <col min="18" max="18" width="14.3" customWidth="true"/>
+    <col min="8" max="9" width="17.7" customWidth="true"/>
+    <col min="10" max="10" width="15" customWidth="true"/>
+    <col min="11" max="11" width="15.7" customWidth="true"/>
+    <col min="12" max="12" width="16.4" customWidth="true"/>
+    <col min="13" max="13" width="16.2" customWidth="true"/>
+    <col min="14" max="14" width="16.9" customWidth="true"/>
+    <col min="15" max="15" width="17.1" customWidth="true"/>
+    <col min="16" max="16" width="15.8" customWidth="true"/>
+    <col min="17" max="17" width="13.5" customWidth="true"/>
+    <col min="18" max="18" width="16.2" customWidth="true"/>
+    <col min="19" max="19" width="14.3" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1096,10 +1102,13 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1108,10 +1117,10 @@
         <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>255000</v>
@@ -1122,17 +1131,17 @@
       <c r="H2">
         <v>50000</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
         <v>50000</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>700000</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1147,15 +1156,18 @@
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>125000</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>125000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="erma@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="erma@primakara.ac.id" tooltip="mailto:erma@primakara.ac.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>